<commit_message>
update for schedule in 2 week
</commit_message>
<xml_diff>
--- a/S1C1_ホアンクイハオ_MTK-RL78G14プログラム課題スケジュール表C3012.Rev1.xlsx
+++ b/S1C1_ホアンクイハオ_MTK-RL78G14プログラム課題スケジュール表C3012.Rev1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E4C1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E4C1\Desktop\Temperature Sr\Temperature-with-renesas-CS-IDE-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
   <si>
     <t>S1C1</t>
     <phoneticPr fontId="1"/>
@@ -385,6 +385,23 @@
     </rPh>
     <rPh sb="379" eb="380">
       <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>担当者のコメント</t>
+    <rPh sb="0" eb="2">
+      <t>タントウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>シャ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お客様のフィードバック</t>
+    <rPh sb="1" eb="3">
+      <t>キャクサマ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1169,7 +1186,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1443,6 +1460,138 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="5" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="8" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="9" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="3" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="6" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="6" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="3" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="34" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="34" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="35" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="34" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1455,6 +1604,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1470,6 +1622,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1479,160 +1640,37 @@
     <xf numFmtId="176" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="27" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="34" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="35" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="34" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="34" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="21" xfId="8" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="9" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="3" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="6" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="6" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="21" xfId="3" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1949,13 +1987,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BE78"/>
+  <dimension ref="A1:BE84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="AN47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="AL43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AQ44" sqref="AQ44"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2005,110 +2043,110 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="109"/>
+      <c r="C1" s="115"/>
     </row>
     <row r="2" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="118"/>
     </row>
     <row r="3" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="111"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="118"/>
     </row>
     <row r="4" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="112"/>
-      <c r="C4" s="111"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="118"/>
     </row>
     <row r="5" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="145" t="s">
+      <c r="B5" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="145" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="101" t="s">
+      <c r="E5" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="99"/>
-      <c r="V5" s="127" t="s">
+      <c r="G5" s="144"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="144"/>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="144"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="144"/>
+      <c r="S5" s="144"/>
+      <c r="T5" s="144"/>
+      <c r="U5" s="144"/>
+      <c r="V5" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="95"/>
-      <c r="X5" s="95"/>
-      <c r="Y5" s="95"/>
-      <c r="Z5" s="95"/>
-      <c r="AA5" s="95"/>
-      <c r="AB5" s="95"/>
-      <c r="AC5" s="95"/>
-      <c r="AD5" s="95"/>
-      <c r="AE5" s="95"/>
-      <c r="AF5" s="95"/>
-      <c r="AG5" s="95"/>
-      <c r="AH5" s="95"/>
-      <c r="AI5" s="95"/>
-      <c r="AJ5" s="95"/>
-      <c r="AK5" s="95"/>
-      <c r="AL5" s="95"/>
-      <c r="AM5" s="95"/>
-      <c r="AN5" s="95"/>
-      <c r="AO5" s="95"/>
-      <c r="AP5" s="95"/>
-      <c r="AQ5" s="95"/>
-      <c r="AR5" s="95"/>
-      <c r="AS5" s="95"/>
-      <c r="AT5" s="95"/>
-      <c r="AU5" s="95"/>
-      <c r="AV5" s="95"/>
-      <c r="AW5" s="95"/>
-      <c r="AX5" s="95"/>
-      <c r="AY5" s="95"/>
-      <c r="AZ5" s="95"/>
-      <c r="BA5" s="139" t="s">
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140"/>
+      <c r="AA5" s="140"/>
+      <c r="AB5" s="140"/>
+      <c r="AC5" s="140"/>
+      <c r="AD5" s="140"/>
+      <c r="AE5" s="140"/>
+      <c r="AF5" s="140"/>
+      <c r="AG5" s="140"/>
+      <c r="AH5" s="140"/>
+      <c r="AI5" s="140"/>
+      <c r="AJ5" s="140"/>
+      <c r="AK5" s="140"/>
+      <c r="AL5" s="140"/>
+      <c r="AM5" s="140"/>
+      <c r="AN5" s="140"/>
+      <c r="AO5" s="140"/>
+      <c r="AP5" s="140"/>
+      <c r="AQ5" s="140"/>
+      <c r="AR5" s="140"/>
+      <c r="AS5" s="140"/>
+      <c r="AT5" s="140"/>
+      <c r="AU5" s="140"/>
+      <c r="AV5" s="140"/>
+      <c r="AW5" s="140"/>
+      <c r="AX5" s="140"/>
+      <c r="AY5" s="140"/>
+      <c r="AZ5" s="140"/>
+      <c r="BA5" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="BB5" s="137"/>
-      <c r="BC5" s="137"/>
-      <c r="BD5" s="137"/>
-      <c r="BE5" s="138"/>
+      <c r="BB5" s="111"/>
+      <c r="BC5" s="111"/>
+      <c r="BD5" s="111"/>
+      <c r="BE5" s="112"/>
     </row>
     <row r="6" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="102"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="150"/>
       <c r="F6" s="38">
         <v>14</v>
       </c>
@@ -2154,7 +2192,7 @@
       <c r="T6" s="4">
         <v>28</v>
       </c>
-      <c r="U6" s="123">
+      <c r="U6" s="91">
         <v>29</v>
       </c>
       <c r="V6" s="38">
@@ -2247,8 +2285,8 @@
       <c r="AY6" s="4">
         <v>30</v>
       </c>
-      <c r="AZ6" s="123"/>
-      <c r="BA6" s="150">
+      <c r="AZ6" s="91"/>
+      <c r="BA6" s="109">
         <v>1</v>
       </c>
       <c r="BB6" s="4">
@@ -2265,11 +2303,11 @@
       </c>
     </row>
     <row r="7" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="115"/>
-      <c r="C7" s="117"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="133"/>
       <c r="D7" s="47"/>
       <c r="E7" s="64"/>
       <c r="F7" s="46"/>
@@ -2290,7 +2328,7 @@
       <c r="S7" s="27"/>
       <c r="T7" s="27"/>
       <c r="U7" s="27"/>
-      <c r="V7" s="128"/>
+      <c r="V7" s="95"/>
       <c r="W7" s="27"/>
       <c r="X7" s="27"/>
       <c r="Y7" s="27"/>
@@ -2328,11 +2366,11 @@
       <c r="BE7" s="27"/>
     </row>
     <row r="8" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A8" s="92"/>
+      <c r="A8" s="136"/>
       <c r="B8" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="114" t="s">
+      <c r="C8" s="131" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="25" t="s">
@@ -2355,48 +2393,48 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="U8" s="124"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="7"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="124"/>
-      <c r="Z8" s="124"/>
-      <c r="AA8" s="124"/>
-      <c r="AB8" s="124"/>
-      <c r="AC8" s="124"/>
+      <c r="Y8" s="92"/>
+      <c r="Z8" s="92"/>
+      <c r="AA8" s="92"/>
+      <c r="AB8" s="92"/>
+      <c r="AC8" s="92"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
-      <c r="AF8" s="124"/>
-      <c r="AG8" s="124"/>
-      <c r="AH8" s="124"/>
-      <c r="AI8" s="124"/>
-      <c r="AJ8" s="124"/>
+      <c r="AF8" s="92"/>
+      <c r="AG8" s="92"/>
+      <c r="AH8" s="92"/>
+      <c r="AI8" s="92"/>
+      <c r="AJ8" s="92"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
-      <c r="AM8" s="124"/>
-      <c r="AN8" s="124"/>
-      <c r="AO8" s="129"/>
-      <c r="AP8" s="124"/>
-      <c r="AQ8" s="124"/>
+      <c r="AM8" s="92"/>
+      <c r="AN8" s="92"/>
+      <c r="AO8" s="96"/>
+      <c r="AP8" s="92"/>
+      <c r="AQ8" s="92"/>
       <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
-      <c r="AT8" s="124"/>
-      <c r="AU8" s="124"/>
-      <c r="AV8" s="124"/>
-      <c r="AW8" s="124"/>
-      <c r="AX8" s="124"/>
+      <c r="AT8" s="92"/>
+      <c r="AU8" s="92"/>
+      <c r="AV8" s="92"/>
+      <c r="AW8" s="92"/>
+      <c r="AX8" s="92"/>
       <c r="AY8" s="3"/>
       <c r="AZ8" s="3"/>
-      <c r="BA8" s="124"/>
-      <c r="BB8" s="124"/>
-      <c r="BC8" s="124"/>
-      <c r="BD8" s="124"/>
-      <c r="BE8" s="124"/>
+      <c r="BA8" s="92"/>
+      <c r="BB8" s="92"/>
+      <c r="BC8" s="92"/>
+      <c r="BD8" s="92"/>
+      <c r="BE8" s="92"/>
     </row>
     <row r="9" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A9" s="92"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="75"/>
-      <c r="C9" s="114"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="26">
         <v>1</v>
       </c>
@@ -2461,9 +2499,9 @@
       <c r="BE9" s="2"/>
     </row>
     <row r="10" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A10" s="92"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="75"/>
-      <c r="C10" s="114" t="s">
+      <c r="C10" s="131" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="25" t="s">
@@ -2481,48 +2519,48 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="U10" s="124"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="7"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
-      <c r="Y10" s="124"/>
-      <c r="Z10" s="124"/>
-      <c r="AA10" s="124"/>
-      <c r="AB10" s="124"/>
-      <c r="AC10" s="124"/>
+      <c r="Y10" s="92"/>
+      <c r="Z10" s="92"/>
+      <c r="AA10" s="92"/>
+      <c r="AB10" s="92"/>
+      <c r="AC10" s="92"/>
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
-      <c r="AF10" s="124"/>
-      <c r="AG10" s="124"/>
-      <c r="AH10" s="124"/>
-      <c r="AI10" s="124"/>
-      <c r="AJ10" s="124"/>
+      <c r="AF10" s="92"/>
+      <c r="AG10" s="92"/>
+      <c r="AH10" s="92"/>
+      <c r="AI10" s="92"/>
+      <c r="AJ10" s="92"/>
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
-      <c r="AM10" s="124"/>
-      <c r="AN10" s="124"/>
-      <c r="AO10" s="129"/>
-      <c r="AP10" s="124"/>
-      <c r="AQ10" s="124"/>
+      <c r="AM10" s="92"/>
+      <c r="AN10" s="92"/>
+      <c r="AO10" s="96"/>
+      <c r="AP10" s="92"/>
+      <c r="AQ10" s="92"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
-      <c r="AT10" s="124"/>
-      <c r="AU10" s="124"/>
-      <c r="AV10" s="124"/>
-      <c r="AW10" s="124"/>
-      <c r="AX10" s="124"/>
+      <c r="AT10" s="92"/>
+      <c r="AU10" s="92"/>
+      <c r="AV10" s="92"/>
+      <c r="AW10" s="92"/>
+      <c r="AX10" s="92"/>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
-      <c r="BA10" s="124"/>
-      <c r="BB10" s="124"/>
-      <c r="BC10" s="124"/>
-      <c r="BD10" s="124"/>
-      <c r="BE10" s="124"/>
+      <c r="BA10" s="92"/>
+      <c r="BB10" s="92"/>
+      <c r="BC10" s="92"/>
+      <c r="BD10" s="92"/>
+      <c r="BE10" s="92"/>
     </row>
     <row r="11" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A11" s="92"/>
+      <c r="A11" s="136"/>
       <c r="B11" s="75"/>
-      <c r="C11" s="114"/>
+      <c r="C11" s="131"/>
       <c r="D11" s="26">
         <v>1</v>
       </c>
@@ -2585,9 +2623,9 @@
       <c r="BE11" s="2"/>
     </row>
     <row r="12" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A12" s="92"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="117"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="133"/>
       <c r="D12" s="78"/>
       <c r="E12" s="58"/>
       <c r="F12" s="46"/>
@@ -2606,7 +2644,7 @@
       <c r="S12" s="27"/>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
-      <c r="V12" s="128"/>
+      <c r="V12" s="95"/>
       <c r="W12" s="27"/>
       <c r="X12" s="27"/>
       <c r="Y12" s="27"/>
@@ -2644,7 +2682,7 @@
       <c r="BE12" s="27"/>
     </row>
     <row r="13" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="76"/>
       <c r="C13" s="44"/>
       <c r="D13" s="43"/>
@@ -2665,7 +2703,7 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
-      <c r="V13" s="130"/>
+      <c r="V13" s="97"/>
       <c r="W13" s="44"/>
       <c r="X13" s="44"/>
       <c r="Y13" s="44"/>
@@ -2703,11 +2741,11 @@
       <c r="BE13" s="44"/>
     </row>
     <row r="14" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="131" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="25" t="s">
@@ -2742,48 +2780,48 @@
       <c r="R14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="124"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="7"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
-      <c r="Y14" s="124"/>
-      <c r="Z14" s="124"/>
-      <c r="AA14" s="124"/>
-      <c r="AB14" s="124"/>
-      <c r="AC14" s="124"/>
+      <c r="Y14" s="92"/>
+      <c r="Z14" s="92"/>
+      <c r="AA14" s="92"/>
+      <c r="AB14" s="92"/>
+      <c r="AC14" s="92"/>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
-      <c r="AF14" s="124"/>
-      <c r="AG14" s="124"/>
-      <c r="AH14" s="124"/>
-      <c r="AI14" s="124"/>
-      <c r="AJ14" s="124"/>
+      <c r="AF14" s="92"/>
+      <c r="AG14" s="92"/>
+      <c r="AH14" s="92"/>
+      <c r="AI14" s="92"/>
+      <c r="AJ14" s="92"/>
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
-      <c r="AM14" s="124"/>
-      <c r="AN14" s="124"/>
-      <c r="AO14" s="129"/>
-      <c r="AP14" s="124"/>
-      <c r="AQ14" s="124"/>
+      <c r="AM14" s="92"/>
+      <c r="AN14" s="92"/>
+      <c r="AO14" s="96"/>
+      <c r="AP14" s="92"/>
+      <c r="AQ14" s="92"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
-      <c r="AT14" s="124"/>
-      <c r="AU14" s="124"/>
-      <c r="AV14" s="124"/>
-      <c r="AW14" s="124"/>
-      <c r="AX14" s="124"/>
+      <c r="AT14" s="92"/>
+      <c r="AU14" s="92"/>
+      <c r="AV14" s="92"/>
+      <c r="AW14" s="92"/>
+      <c r="AX14" s="92"/>
       <c r="AY14" s="3"/>
       <c r="AZ14" s="3"/>
-      <c r="BA14" s="124"/>
-      <c r="BB14" s="124"/>
-      <c r="BC14" s="124"/>
-      <c r="BD14" s="124"/>
-      <c r="BE14" s="124"/>
+      <c r="BA14" s="92"/>
+      <c r="BB14" s="92"/>
+      <c r="BC14" s="92"/>
+      <c r="BD14" s="92"/>
+      <c r="BE14" s="92"/>
     </row>
     <row r="15" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
+      <c r="A15" s="137"/>
       <c r="B15" s="76"/>
-      <c r="C15" s="114"/>
+      <c r="C15" s="131"/>
       <c r="D15" s="26">
         <v>1</v>
       </c>
@@ -2856,9 +2894,9 @@
       <c r="BE15" s="2"/>
     </row>
     <row r="16" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
+      <c r="A16" s="137"/>
       <c r="B16" s="76"/>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="131" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="25" t="s">
@@ -2877,48 +2915,48 @@
       <c r="S16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="U16" s="124"/>
+      <c r="U16" s="92"/>
       <c r="V16" s="7"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="124"/>
-      <c r="Z16" s="124"/>
-      <c r="AA16" s="124"/>
-      <c r="AB16" s="124"/>
-      <c r="AC16" s="124"/>
+      <c r="Y16" s="92"/>
+      <c r="Z16" s="92"/>
+      <c r="AA16" s="92"/>
+      <c r="AB16" s="92"/>
+      <c r="AC16" s="92"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
-      <c r="AF16" s="124"/>
-      <c r="AG16" s="124"/>
-      <c r="AH16" s="124"/>
-      <c r="AI16" s="124"/>
-      <c r="AJ16" s="124"/>
+      <c r="AF16" s="92"/>
+      <c r="AG16" s="92"/>
+      <c r="AH16" s="92"/>
+      <c r="AI16" s="92"/>
+      <c r="AJ16" s="92"/>
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
-      <c r="AM16" s="124"/>
-      <c r="AN16" s="124"/>
-      <c r="AO16" s="129"/>
-      <c r="AP16" s="124"/>
-      <c r="AQ16" s="124"/>
+      <c r="AM16" s="92"/>
+      <c r="AN16" s="92"/>
+      <c r="AO16" s="96"/>
+      <c r="AP16" s="92"/>
+      <c r="AQ16" s="92"/>
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
-      <c r="AT16" s="124"/>
-      <c r="AU16" s="124"/>
-      <c r="AV16" s="124"/>
-      <c r="AW16" s="124"/>
-      <c r="AX16" s="124"/>
+      <c r="AT16" s="92"/>
+      <c r="AU16" s="92"/>
+      <c r="AV16" s="92"/>
+      <c r="AW16" s="92"/>
+      <c r="AX16" s="92"/>
       <c r="AY16" s="3"/>
       <c r="AZ16" s="3"/>
-      <c r="BA16" s="124"/>
-      <c r="BB16" s="124"/>
-      <c r="BC16" s="124"/>
-      <c r="BD16" s="124"/>
-      <c r="BE16" s="124"/>
+      <c r="BA16" s="92"/>
+      <c r="BB16" s="92"/>
+      <c r="BC16" s="92"/>
+      <c r="BD16" s="92"/>
+      <c r="BE16" s="92"/>
     </row>
     <row r="17" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
+      <c r="A17" s="137"/>
       <c r="B17" s="76"/>
-      <c r="C17" s="114"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="26">
         <v>1</v>
       </c>
@@ -2981,7 +3019,7 @@
       <c r="BE17" s="2"/>
     </row>
     <row r="18" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="93"/>
+      <c r="A18" s="137"/>
       <c r="B18" s="76"/>
       <c r="C18" s="44"/>
       <c r="D18" s="77"/>
@@ -3002,7 +3040,7 @@
       <c r="S18" s="44"/>
       <c r="T18" s="44"/>
       <c r="U18" s="44"/>
-      <c r="V18" s="130"/>
+      <c r="V18" s="97"/>
       <c r="W18" s="44"/>
       <c r="X18" s="44"/>
       <c r="Y18" s="44"/>
@@ -3040,9 +3078,9 @@
       <c r="BE18" s="44"/>
     </row>
     <row r="19" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="93"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="119"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="50"/>
       <c r="E19" s="63"/>
       <c r="F19" s="51"/>
@@ -3080,7 +3118,7 @@
       <c r="AL19" s="52"/>
       <c r="AM19" s="52"/>
       <c r="AN19" s="52"/>
-      <c r="AO19" s="131"/>
+      <c r="AO19" s="98"/>
       <c r="AP19" s="52"/>
       <c r="AQ19" s="52"/>
       <c r="AR19" s="52"/>
@@ -3099,11 +3137,11 @@
       <c r="BE19" s="52"/>
     </row>
     <row r="20" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="121" t="s">
+      <c r="A20" s="137"/>
+      <c r="B20" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="105" t="s">
+      <c r="C20" s="129" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -3121,50 +3159,50 @@
       <c r="T20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U20" s="125" t="s">
+      <c r="U20" s="93" t="s">
         <v>29</v>
       </c>
       <c r="V20" s="7"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="124"/>
-      <c r="Z20" s="124"/>
-      <c r="AA20" s="124"/>
-      <c r="AB20" s="124"/>
-      <c r="AC20" s="124"/>
+      <c r="Y20" s="92"/>
+      <c r="Z20" s="92"/>
+      <c r="AA20" s="92"/>
+      <c r="AB20" s="92"/>
+      <c r="AC20" s="92"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3"/>
-      <c r="AF20" s="124"/>
-      <c r="AG20" s="124"/>
-      <c r="AH20" s="124"/>
-      <c r="AI20" s="124"/>
-      <c r="AJ20" s="124"/>
+      <c r="AF20" s="92"/>
+      <c r="AG20" s="92"/>
+      <c r="AH20" s="92"/>
+      <c r="AI20" s="92"/>
+      <c r="AJ20" s="92"/>
       <c r="AK20" s="3"/>
       <c r="AL20" s="3"/>
-      <c r="AM20" s="124"/>
-      <c r="AN20" s="124"/>
-      <c r="AO20" s="129"/>
-      <c r="AP20" s="124"/>
-      <c r="AQ20" s="124"/>
+      <c r="AM20" s="92"/>
+      <c r="AN20" s="92"/>
+      <c r="AO20" s="96"/>
+      <c r="AP20" s="92"/>
+      <c r="AQ20" s="92"/>
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
-      <c r="AT20" s="124"/>
-      <c r="AU20" s="124"/>
-      <c r="AV20" s="124"/>
-      <c r="AW20" s="124"/>
-      <c r="AX20" s="124"/>
+      <c r="AT20" s="92"/>
+      <c r="AU20" s="92"/>
+      <c r="AV20" s="92"/>
+      <c r="AW20" s="92"/>
+      <c r="AX20" s="92"/>
       <c r="AY20" s="3"/>
       <c r="AZ20" s="3"/>
-      <c r="BA20" s="124"/>
-      <c r="BB20" s="124"/>
-      <c r="BC20" s="124"/>
-      <c r="BD20" s="124"/>
-      <c r="BE20" s="124"/>
+      <c r="BA20" s="92"/>
+      <c r="BB20" s="92"/>
+      <c r="BC20" s="92"/>
+      <c r="BD20" s="92"/>
+      <c r="BE20" s="92"/>
     </row>
     <row r="21" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="105"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="128"/>
+      <c r="C21" s="129"/>
       <c r="D21" s="26">
         <v>1</v>
       </c>
@@ -3229,9 +3267,9 @@
       <c r="BE21" s="2"/>
     </row>
     <row r="22" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="105" t="s">
+      <c r="A22" s="137"/>
+      <c r="B22" s="128"/>
+      <c r="C22" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -3246,52 +3284,52 @@
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
-      <c r="U22" s="124"/>
-      <c r="V22" s="132" t="s">
+      <c r="U22" s="92"/>
+      <c r="V22" s="99" t="s">
         <v>21</v>
       </c>
       <c r="W22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X22" s="3"/>
-      <c r="Y22" s="124"/>
-      <c r="Z22" s="124"/>
-      <c r="AA22" s="124"/>
-      <c r="AB22" s="124"/>
-      <c r="AC22" s="124"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="92"/>
+      <c r="AB22" s="92"/>
+      <c r="AC22" s="92"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
-      <c r="AF22" s="124"/>
-      <c r="AG22" s="124"/>
-      <c r="AH22" s="124"/>
-      <c r="AI22" s="124"/>
-      <c r="AJ22" s="124"/>
+      <c r="AF22" s="92"/>
+      <c r="AG22" s="92"/>
+      <c r="AH22" s="92"/>
+      <c r="AI22" s="92"/>
+      <c r="AJ22" s="92"/>
       <c r="AK22" s="3"/>
       <c r="AL22" s="3"/>
-      <c r="AM22" s="124"/>
-      <c r="AN22" s="124"/>
-      <c r="AO22" s="129"/>
-      <c r="AP22" s="124"/>
-      <c r="AQ22" s="124"/>
+      <c r="AM22" s="92"/>
+      <c r="AN22" s="92"/>
+      <c r="AO22" s="96"/>
+      <c r="AP22" s="92"/>
+      <c r="AQ22" s="92"/>
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
-      <c r="AT22" s="124"/>
-      <c r="AU22" s="124"/>
-      <c r="AV22" s="124"/>
-      <c r="AW22" s="124"/>
-      <c r="AX22" s="124"/>
+      <c r="AT22" s="92"/>
+      <c r="AU22" s="92"/>
+      <c r="AV22" s="92"/>
+      <c r="AW22" s="92"/>
+      <c r="AX22" s="92"/>
       <c r="AY22" s="3"/>
       <c r="AZ22" s="3"/>
-      <c r="BA22" s="124"/>
-      <c r="BB22" s="124"/>
-      <c r="BC22" s="124"/>
-      <c r="BD22" s="124"/>
-      <c r="BE22" s="124"/>
+      <c r="BA22" s="92"/>
+      <c r="BB22" s="92"/>
+      <c r="BC22" s="92"/>
+      <c r="BD22" s="92"/>
+      <c r="BE22" s="92"/>
     </row>
     <row r="23" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="105"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="129"/>
       <c r="D23" s="26">
         <v>0</v>
       </c>
@@ -3354,9 +3392,9 @@
       <c r="BE23" s="2"/>
     </row>
     <row r="24" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="93"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="105" t="s">
+      <c r="A24" s="137"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="129" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -3371,52 +3409,52 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
-      <c r="U24" s="124"/>
+      <c r="U24" s="92"/>
       <c r="V24" s="7"/>
       <c r="W24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X24" s="3"/>
-      <c r="Y24" s="125" t="s">
+      <c r="Y24" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="Z24" s="124"/>
-      <c r="AA24" s="124"/>
-      <c r="AB24" s="124"/>
-      <c r="AC24" s="124"/>
+      <c r="Z24" s="92"/>
+      <c r="AA24" s="92"/>
+      <c r="AB24" s="92"/>
+      <c r="AC24" s="92"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
-      <c r="AF24" s="124"/>
-      <c r="AG24" s="124"/>
-      <c r="AH24" s="124"/>
-      <c r="AI24" s="124"/>
-      <c r="AJ24" s="124"/>
+      <c r="AF24" s="92"/>
+      <c r="AG24" s="92"/>
+      <c r="AH24" s="92"/>
+      <c r="AI24" s="92"/>
+      <c r="AJ24" s="92"/>
       <c r="AK24" s="3"/>
       <c r="AL24" s="3"/>
-      <c r="AM24" s="124"/>
-      <c r="AN24" s="124"/>
-      <c r="AO24" s="129"/>
-      <c r="AP24" s="124"/>
-      <c r="AQ24" s="124"/>
+      <c r="AM24" s="92"/>
+      <c r="AN24" s="92"/>
+      <c r="AO24" s="96"/>
+      <c r="AP24" s="92"/>
+      <c r="AQ24" s="92"/>
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
-      <c r="AT24" s="124"/>
-      <c r="AU24" s="124"/>
-      <c r="AV24" s="124"/>
-      <c r="AW24" s="124"/>
-      <c r="AX24" s="124"/>
+      <c r="AT24" s="92"/>
+      <c r="AU24" s="92"/>
+      <c r="AV24" s="92"/>
+      <c r="AW24" s="92"/>
+      <c r="AX24" s="92"/>
       <c r="AY24" s="3"/>
       <c r="AZ24" s="3"/>
-      <c r="BA24" s="124"/>
-      <c r="BB24" s="124"/>
-      <c r="BC24" s="124"/>
-      <c r="BD24" s="124"/>
-      <c r="BE24" s="124"/>
+      <c r="BA24" s="92"/>
+      <c r="BB24" s="92"/>
+      <c r="BC24" s="92"/>
+      <c r="BD24" s="92"/>
+      <c r="BE24" s="92"/>
     </row>
     <row r="25" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="93"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="105"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="129"/>
       <c r="D25" s="26">
         <v>1</v>
       </c>
@@ -3479,9 +3517,9 @@
       <c r="BE25" s="2"/>
     </row>
     <row r="26" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="93"/>
-      <c r="B26" s="122"/>
-      <c r="C26" s="105" t="s">
+      <c r="A26" s="137"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="25" t="s">
@@ -3496,52 +3534,52 @@
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
-      <c r="U26" s="124"/>
+      <c r="U26" s="92"/>
       <c r="V26" s="7"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="124" t="s">
+      <c r="Y26" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="Z26" s="125" t="s">
+      <c r="Z26" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="AA26" s="124"/>
-      <c r="AB26" s="124"/>
-      <c r="AC26" s="124"/>
+      <c r="AA26" s="92"/>
+      <c r="AB26" s="92"/>
+      <c r="AC26" s="92"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="124"/>
-      <c r="AG26" s="124"/>
-      <c r="AH26" s="124"/>
-      <c r="AI26" s="124"/>
-      <c r="AJ26" s="124"/>
+      <c r="AF26" s="92"/>
+      <c r="AG26" s="92"/>
+      <c r="AH26" s="92"/>
+      <c r="AI26" s="92"/>
+      <c r="AJ26" s="92"/>
       <c r="AK26" s="3"/>
       <c r="AL26" s="3"/>
-      <c r="AM26" s="124"/>
-      <c r="AN26" s="124"/>
-      <c r="AO26" s="129"/>
-      <c r="AP26" s="124"/>
-      <c r="AQ26" s="124"/>
+      <c r="AM26" s="92"/>
+      <c r="AN26" s="92"/>
+      <c r="AO26" s="96"/>
+      <c r="AP26" s="92"/>
+      <c r="AQ26" s="92"/>
       <c r="AR26" s="3"/>
       <c r="AS26" s="3"/>
-      <c r="AT26" s="124"/>
-      <c r="AU26" s="124"/>
-      <c r="AV26" s="124"/>
-      <c r="AW26" s="124"/>
-      <c r="AX26" s="124"/>
+      <c r="AT26" s="92"/>
+      <c r="AU26" s="92"/>
+      <c r="AV26" s="92"/>
+      <c r="AW26" s="92"/>
+      <c r="AX26" s="92"/>
       <c r="AY26" s="3"/>
       <c r="AZ26" s="3"/>
-      <c r="BA26" s="124"/>
-      <c r="BB26" s="124"/>
-      <c r="BC26" s="124"/>
-      <c r="BD26" s="124"/>
-      <c r="BE26" s="124"/>
+      <c r="BA26" s="92"/>
+      <c r="BB26" s="92"/>
+      <c r="BC26" s="92"/>
+      <c r="BD26" s="92"/>
+      <c r="BE26" s="92"/>
     </row>
     <row r="27" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="93"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="105"/>
+      <c r="A27" s="137"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="129"/>
       <c r="D27" s="26">
         <v>0</v>
       </c>
@@ -3568,7 +3606,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="2"/>
-      <c r="Z27" s="133">
+      <c r="Z27" s="100">
         <v>1</v>
       </c>
       <c r="AA27" s="2"/>
@@ -3604,9 +3642,9 @@
       <c r="BE27" s="2"/>
     </row>
     <row r="28" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="93"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="105" t="s">
+      <c r="A28" s="137"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="129" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -3621,54 +3659,54 @@
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
-      <c r="U28" s="124"/>
+      <c r="U28" s="92"/>
       <c r="V28" s="7"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-      <c r="Y28" s="124"/>
-      <c r="Z28" s="124"/>
-      <c r="AA28" s="125" t="s">
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="92"/>
+      <c r="AA28" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="AB28" s="125" t="s">
+      <c r="AB28" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="AC28" s="125" t="s">
+      <c r="AC28" s="93" t="s">
         <v>35</v>
       </c>
       <c r="AD28" s="3"/>
       <c r="AE28" s="3"/>
-      <c r="AF28" s="124"/>
-      <c r="AG28" s="124"/>
-      <c r="AH28" s="124"/>
-      <c r="AI28" s="124"/>
-      <c r="AJ28" s="124"/>
+      <c r="AF28" s="92"/>
+      <c r="AG28" s="92"/>
+      <c r="AH28" s="92"/>
+      <c r="AI28" s="92"/>
+      <c r="AJ28" s="92"/>
       <c r="AK28" s="3"/>
       <c r="AL28" s="3"/>
-      <c r="AM28" s="124"/>
-      <c r="AN28" s="124"/>
-      <c r="AO28" s="129"/>
-      <c r="AP28" s="124"/>
-      <c r="AQ28" s="124"/>
+      <c r="AM28" s="92"/>
+      <c r="AN28" s="92"/>
+      <c r="AO28" s="96"/>
+      <c r="AP28" s="92"/>
+      <c r="AQ28" s="92"/>
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
-      <c r="AT28" s="124"/>
-      <c r="AU28" s="124"/>
-      <c r="AV28" s="124"/>
-      <c r="AW28" s="124"/>
-      <c r="AX28" s="136"/>
+      <c r="AT28" s="92"/>
+      <c r="AU28" s="92"/>
+      <c r="AV28" s="92"/>
+      <c r="AW28" s="92"/>
+      <c r="AX28" s="103"/>
       <c r="AY28" s="3"/>
       <c r="AZ28" s="3"/>
-      <c r="BA28" s="124"/>
-      <c r="BB28" s="124"/>
-      <c r="BC28" s="124"/>
-      <c r="BD28" s="124"/>
-      <c r="BE28" s="136"/>
+      <c r="BA28" s="92"/>
+      <c r="BB28" s="92"/>
+      <c r="BC28" s="92"/>
+      <c r="BD28" s="92"/>
+      <c r="BE28" s="103"/>
     </row>
     <row r="29" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="105"/>
+      <c r="A29" s="137"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="129"/>
       <c r="D29" s="26">
         <v>1</v>
       </c>
@@ -3696,7 +3734,7 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
-      <c r="AA29" s="133">
+      <c r="AA29" s="100">
         <v>1</v>
       </c>
       <c r="AB29" s="21">
@@ -3735,9 +3773,9 @@
       <c r="BE29" s="2"/>
     </row>
     <row r="30" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="105" t="s">
+      <c r="A30" s="137"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -3752,50 +3790,50 @@
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
-      <c r="U30" s="124"/>
+      <c r="U30" s="92"/>
       <c r="V30" s="7"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="124"/>
-      <c r="Z30" s="124"/>
-      <c r="AA30" s="124"/>
-      <c r="AB30" s="124"/>
-      <c r="AC30" s="124"/>
+      <c r="Y30" s="92"/>
+      <c r="Z30" s="92"/>
+      <c r="AA30" s="92"/>
+      <c r="AB30" s="92"/>
+      <c r="AC30" s="92"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
-      <c r="AF30" s="125" t="s">
+      <c r="AF30" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="AG30" s="124"/>
-      <c r="AH30" s="124"/>
-      <c r="AI30" s="124"/>
-      <c r="AJ30" s="124"/>
+      <c r="AG30" s="92"/>
+      <c r="AH30" s="92"/>
+      <c r="AI30" s="92"/>
+      <c r="AJ30" s="92"/>
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
-      <c r="AM30" s="124"/>
-      <c r="AN30" s="124"/>
-      <c r="AO30" s="129"/>
-      <c r="AP30" s="124"/>
-      <c r="AQ30" s="124"/>
+      <c r="AM30" s="92"/>
+      <c r="AN30" s="92"/>
+      <c r="AO30" s="96"/>
+      <c r="AP30" s="92"/>
+      <c r="AQ30" s="92"/>
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
-      <c r="AT30" s="124"/>
-      <c r="AU30" s="124"/>
-      <c r="AV30" s="124"/>
-      <c r="AW30" s="124"/>
-      <c r="AX30" s="124"/>
+      <c r="AT30" s="92"/>
+      <c r="AU30" s="92"/>
+      <c r="AV30" s="92"/>
+      <c r="AW30" s="92"/>
+      <c r="AX30" s="92"/>
       <c r="AY30" s="3"/>
       <c r="AZ30" s="3"/>
-      <c r="BA30" s="124"/>
-      <c r="BB30" s="124"/>
-      <c r="BC30" s="124"/>
-      <c r="BD30" s="124"/>
-      <c r="BE30" s="124"/>
+      <c r="BA30" s="92"/>
+      <c r="BB30" s="92"/>
+      <c r="BC30" s="92"/>
+      <c r="BD30" s="92"/>
+      <c r="BE30" s="92"/>
     </row>
     <row r="31" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="93"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="105"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="129"/>
       <c r="D31" s="26">
         <v>0</v>
       </c>
@@ -3858,9 +3896,9 @@
       <c r="BE31" s="2"/>
     </row>
     <row r="32" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="105" t="s">
+      <c r="A32" s="137"/>
+      <c r="B32" s="128"/>
+      <c r="C32" s="129" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -3875,50 +3913,50 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
-      <c r="U32" s="124"/>
+      <c r="U32" s="92"/>
       <c r="V32" s="7"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="124"/>
-      <c r="Z32" s="124"/>
-      <c r="AA32" s="124"/>
-      <c r="AB32" s="124"/>
-      <c r="AC32" s="124"/>
+      <c r="Y32" s="92"/>
+      <c r="Z32" s="92"/>
+      <c r="AA32" s="92"/>
+      <c r="AB32" s="92"/>
+      <c r="AC32" s="92"/>
       <c r="AD32" s="3"/>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="124"/>
-      <c r="AG32" s="125" t="s">
+      <c r="AF32" s="92"/>
+      <c r="AG32" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="AH32" s="124"/>
-      <c r="AI32" s="124"/>
-      <c r="AJ32" s="124"/>
+      <c r="AH32" s="92"/>
+      <c r="AI32" s="92"/>
+      <c r="AJ32" s="92"/>
       <c r="AK32" s="3"/>
       <c r="AL32" s="3"/>
-      <c r="AM32" s="124"/>
-      <c r="AN32" s="124"/>
-      <c r="AO32" s="129"/>
-      <c r="AP32" s="124"/>
-      <c r="AQ32" s="124"/>
+      <c r="AM32" s="92"/>
+      <c r="AN32" s="92"/>
+      <c r="AO32" s="96"/>
+      <c r="AP32" s="92"/>
+      <c r="AQ32" s="92"/>
       <c r="AR32" s="3"/>
       <c r="AS32" s="3"/>
-      <c r="AT32" s="124"/>
-      <c r="AU32" s="124"/>
-      <c r="AV32" s="124"/>
-      <c r="AW32" s="124"/>
-      <c r="AX32" s="124"/>
+      <c r="AT32" s="92"/>
+      <c r="AU32" s="92"/>
+      <c r="AV32" s="92"/>
+      <c r="AW32" s="92"/>
+      <c r="AX32" s="92"/>
       <c r="AY32" s="3"/>
       <c r="AZ32" s="3"/>
-      <c r="BA32" s="124"/>
-      <c r="BB32" s="124"/>
-      <c r="BC32" s="124"/>
-      <c r="BD32" s="124"/>
-      <c r="BE32" s="124"/>
+      <c r="BA32" s="92"/>
+      <c r="BB32" s="92"/>
+      <c r="BC32" s="92"/>
+      <c r="BD32" s="92"/>
+      <c r="BE32" s="92"/>
     </row>
     <row r="33" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="93"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="105"/>
+      <c r="A33" s="137"/>
+      <c r="B33" s="128"/>
+      <c r="C33" s="129"/>
       <c r="D33" s="26">
         <v>0</v>
       </c>
@@ -3981,9 +4019,9 @@
       <c r="BE33" s="2"/>
     </row>
     <row r="34" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="93"/>
-      <c r="B34" s="122"/>
-      <c r="C34" s="105" t="s">
+      <c r="A34" s="137"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="25" t="s">
@@ -3998,52 +4036,52 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
-      <c r="U34" s="124"/>
+      <c r="U34" s="92"/>
       <c r="V34" s="7"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="124"/>
-      <c r="Z34" s="124"/>
-      <c r="AA34" s="124"/>
-      <c r="AB34" s="124"/>
-      <c r="AC34" s="124"/>
+      <c r="Y34" s="92"/>
+      <c r="Z34" s="92"/>
+      <c r="AA34" s="92"/>
+      <c r="AB34" s="92"/>
+      <c r="AC34" s="92"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
-      <c r="AF34" s="124"/>
-      <c r="AG34" s="124"/>
-      <c r="AH34" s="125" t="s">
+      <c r="AF34" s="92"/>
+      <c r="AG34" s="92"/>
+      <c r="AH34" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="AI34" s="124" t="s">
+      <c r="AI34" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="AJ34" s="124"/>
+      <c r="AJ34" s="92"/>
       <c r="AK34" s="3"/>
       <c r="AL34" s="3"/>
-      <c r="AM34" s="124"/>
-      <c r="AN34" s="124"/>
-      <c r="AO34" s="129"/>
-      <c r="AP34" s="124"/>
-      <c r="AQ34" s="124"/>
+      <c r="AM34" s="92"/>
+      <c r="AN34" s="92"/>
+      <c r="AO34" s="96"/>
+      <c r="AP34" s="92"/>
+      <c r="AQ34" s="92"/>
       <c r="AR34" s="3"/>
       <c r="AS34" s="3"/>
-      <c r="AT34" s="124"/>
-      <c r="AU34" s="124"/>
-      <c r="AV34" s="124"/>
-      <c r="AW34" s="124"/>
-      <c r="AX34" s="124"/>
+      <c r="AT34" s="92"/>
+      <c r="AU34" s="92"/>
+      <c r="AV34" s="92"/>
+      <c r="AW34" s="92"/>
+      <c r="AX34" s="92"/>
       <c r="AY34" s="3"/>
       <c r="AZ34" s="3"/>
-      <c r="BA34" s="124"/>
-      <c r="BB34" s="124"/>
-      <c r="BC34" s="124"/>
-      <c r="BD34" s="124"/>
-      <c r="BE34" s="124"/>
+      <c r="BA34" s="92"/>
+      <c r="BB34" s="92"/>
+      <c r="BC34" s="92"/>
+      <c r="BD34" s="92"/>
+      <c r="BE34" s="92"/>
     </row>
     <row r="35" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="93"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="105"/>
+      <c r="A35" s="137"/>
+      <c r="B35" s="128"/>
+      <c r="C35" s="129"/>
       <c r="D35" s="26">
         <v>0</v>
       </c>
@@ -4106,9 +4144,9 @@
       <c r="BE35" s="2"/>
     </row>
     <row r="36" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="93"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="105" t="s">
+      <c r="A36" s="137"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="129" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="25" t="s">
@@ -4123,52 +4161,52 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
-      <c r="U36" s="124"/>
+      <c r="U36" s="92"/>
       <c r="V36" s="7"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="124"/>
-      <c r="Z36" s="124"/>
-      <c r="AA36" s="124"/>
-      <c r="AB36" s="124"/>
-      <c r="AC36" s="124"/>
+      <c r="Y36" s="92"/>
+      <c r="Z36" s="92"/>
+      <c r="AA36" s="92"/>
+      <c r="AB36" s="92"/>
+      <c r="AC36" s="92"/>
       <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
-      <c r="AF36" s="124"/>
-      <c r="AG36" s="124"/>
-      <c r="AH36" s="124"/>
-      <c r="AI36" s="125">
+      <c r="AF36" s="92"/>
+      <c r="AG36" s="92"/>
+      <c r="AH36" s="92"/>
+      <c r="AI36" s="93">
         <v>400</v>
       </c>
-      <c r="AJ36" s="125">
+      <c r="AJ36" s="93">
         <v>400</v>
       </c>
       <c r="AK36" s="3"/>
       <c r="AL36" s="3"/>
-      <c r="AM36" s="124"/>
-      <c r="AN36" s="124"/>
-      <c r="AO36" s="129"/>
-      <c r="AP36" s="124"/>
-      <c r="AQ36" s="124"/>
+      <c r="AM36" s="92"/>
+      <c r="AN36" s="92"/>
+      <c r="AO36" s="96"/>
+      <c r="AP36" s="92"/>
+      <c r="AQ36" s="92"/>
       <c r="AR36" s="3"/>
       <c r="AS36" s="3"/>
-      <c r="AT36" s="124"/>
-      <c r="AU36" s="124"/>
-      <c r="AV36" s="124"/>
-      <c r="AW36" s="124"/>
-      <c r="AX36" s="124"/>
+      <c r="AT36" s="92"/>
+      <c r="AU36" s="92"/>
+      <c r="AV36" s="92"/>
+      <c r="AW36" s="92"/>
+      <c r="AX36" s="92"/>
       <c r="AY36" s="3"/>
       <c r="AZ36" s="3"/>
-      <c r="BA36" s="124"/>
-      <c r="BB36" s="124"/>
-      <c r="BC36" s="124"/>
-      <c r="BD36" s="124"/>
-      <c r="BE36" s="124"/>
+      <c r="BA36" s="92"/>
+      <c r="BB36" s="92"/>
+      <c r="BC36" s="92"/>
+      <c r="BD36" s="92"/>
+      <c r="BE36" s="92"/>
     </row>
     <row r="37" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="93"/>
-      <c r="B37" s="122"/>
-      <c r="C37" s="105"/>
+      <c r="A37" s="137"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="129"/>
       <c r="D37" s="26">
         <v>0</v>
       </c>
@@ -4233,9 +4271,9 @@
       <c r="BE37" s="2"/>
     </row>
     <row r="38" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A38" s="93"/>
-      <c r="B38" s="122"/>
-      <c r="C38" s="105" t="s">
+      <c r="A38" s="137"/>
+      <c r="B38" s="128"/>
+      <c r="C38" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="25" t="s">
@@ -4250,52 +4288,52 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
-      <c r="U38" s="124"/>
+      <c r="U38" s="92"/>
       <c r="V38" s="7"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-      <c r="Y38" s="124"/>
-      <c r="Z38" s="124"/>
-      <c r="AA38" s="124"/>
-      <c r="AB38" s="124"/>
-      <c r="AC38" s="124"/>
+      <c r="Y38" s="92"/>
+      <c r="Z38" s="92"/>
+      <c r="AA38" s="92"/>
+      <c r="AB38" s="92"/>
+      <c r="AC38" s="92"/>
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
-      <c r="AF38" s="124"/>
-      <c r="AG38" s="124"/>
-      <c r="AH38" s="124"/>
-      <c r="AI38" s="124"/>
-      <c r="AJ38" s="124"/>
+      <c r="AF38" s="92"/>
+      <c r="AG38" s="92"/>
+      <c r="AH38" s="92"/>
+      <c r="AI38" s="92"/>
+      <c r="AJ38" s="92"/>
       <c r="AK38" s="3"/>
       <c r="AL38" s="3"/>
-      <c r="AM38" s="125" t="s">
+      <c r="AM38" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="AN38" s="124" t="s">
+      <c r="AN38" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="AO38" s="129"/>
-      <c r="AP38" s="124"/>
-      <c r="AQ38" s="124"/>
+      <c r="AO38" s="96"/>
+      <c r="AP38" s="92"/>
+      <c r="AQ38" s="92"/>
       <c r="AR38" s="3"/>
       <c r="AS38" s="3"/>
-      <c r="AT38" s="124"/>
-      <c r="AU38" s="124"/>
-      <c r="AV38" s="124"/>
-      <c r="AW38" s="124"/>
-      <c r="AX38" s="124"/>
+      <c r="AT38" s="92"/>
+      <c r="AU38" s="92"/>
+      <c r="AV38" s="92"/>
+      <c r="AW38" s="92"/>
+      <c r="AX38" s="92"/>
       <c r="AY38" s="3"/>
       <c r="AZ38" s="3"/>
-      <c r="BA38" s="124"/>
-      <c r="BB38" s="124"/>
-      <c r="BC38" s="124"/>
-      <c r="BD38" s="124"/>
-      <c r="BE38" s="124"/>
+      <c r="BA38" s="92"/>
+      <c r="BB38" s="92"/>
+      <c r="BC38" s="92"/>
+      <c r="BD38" s="92"/>
+      <c r="BE38" s="92"/>
     </row>
     <row r="39" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A39" s="93"/>
-      <c r="B39" s="122"/>
-      <c r="C39" s="105"/>
+      <c r="A39" s="137"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="129"/>
       <c r="D39" s="26">
         <v>0</v>
       </c>
@@ -4335,7 +4373,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
-      <c r="AM39" s="134"/>
+      <c r="AM39" s="101"/>
       <c r="AN39" s="2"/>
       <c r="AO39" s="87"/>
       <c r="AP39" s="2"/>
@@ -4356,7 +4394,7 @@
       <c r="BE39" s="2"/>
     </row>
     <row r="40" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A40" s="93"/>
+      <c r="A40" s="137"/>
       <c r="B40" s="73"/>
       <c r="C40" s="74"/>
       <c r="D40" s="50"/>
@@ -4396,7 +4434,7 @@
       <c r="AL40" s="52"/>
       <c r="AM40" s="52"/>
       <c r="AN40" s="52"/>
-      <c r="AO40" s="131"/>
+      <c r="AO40" s="98"/>
       <c r="AP40" s="52"/>
       <c r="AQ40" s="52"/>
       <c r="AR40" s="52"/>
@@ -4415,9 +4453,9 @@
       <c r="BE40" s="53"/>
     </row>
     <row r="41" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A41" s="93"/>
-      <c r="B41" s="106"/>
-      <c r="C41" s="107"/>
+      <c r="A41" s="137"/>
+      <c r="B41" s="124"/>
+      <c r="C41" s="125"/>
       <c r="D41" s="49"/>
       <c r="E41" s="59"/>
       <c r="F41" s="28"/>
@@ -4474,11 +4512,11 @@
       <c r="BE41" s="30"/>
     </row>
     <row r="42" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A42" s="93"/>
-      <c r="B42" s="120" t="s">
+      <c r="A42" s="137"/>
+      <c r="B42" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="105" t="s">
+      <c r="C42" s="129" t="s">
         <v>40</v>
       </c>
       <c r="D42" s="25" t="s">
@@ -4495,48 +4533,48 @@
       <c r="V42" s="7"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-      <c r="Y42" s="124"/>
-      <c r="Z42" s="124"/>
-      <c r="AA42" s="124"/>
-      <c r="AB42" s="124"/>
-      <c r="AC42" s="124"/>
+      <c r="Y42" s="92"/>
+      <c r="Z42" s="92"/>
+      <c r="AA42" s="92"/>
+      <c r="AB42" s="92"/>
+      <c r="AC42" s="92"/>
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
-      <c r="AF42" s="124"/>
-      <c r="AG42" s="124"/>
-      <c r="AH42" s="124"/>
-      <c r="AI42" s="124"/>
-      <c r="AJ42" s="124"/>
+      <c r="AF42" s="92"/>
+      <c r="AG42" s="92"/>
+      <c r="AH42" s="92"/>
+      <c r="AI42" s="92"/>
+      <c r="AJ42" s="92"/>
       <c r="AK42" s="3"/>
       <c r="AL42" s="3"/>
-      <c r="AM42" s="124"/>
-      <c r="AN42" s="125" t="s">
+      <c r="AM42" s="92"/>
+      <c r="AN42" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="AO42" s="129" t="s">
+      <c r="AO42" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="AP42" s="124"/>
-      <c r="AQ42" s="124"/>
+      <c r="AP42" s="92"/>
+      <c r="AQ42" s="92"/>
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
-      <c r="AT42" s="124"/>
-      <c r="AU42" s="124"/>
-      <c r="AV42" s="124"/>
-      <c r="AW42" s="124"/>
-      <c r="AX42" s="124"/>
+      <c r="AT42" s="92"/>
+      <c r="AU42" s="92"/>
+      <c r="AV42" s="92"/>
+      <c r="AW42" s="92"/>
+      <c r="AX42" s="92"/>
       <c r="AY42" s="3"/>
       <c r="AZ42" s="3"/>
       <c r="BA42" s="7"/>
-      <c r="BB42" s="124"/>
-      <c r="BC42" s="124"/>
-      <c r="BD42" s="124"/>
+      <c r="BB42" s="92"/>
+      <c r="BC42" s="92"/>
+      <c r="BD42" s="92"/>
       <c r="BE42" s="8"/>
     </row>
     <row r="43" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A43" s="93"/>
-      <c r="B43" s="120"/>
-      <c r="C43" s="105"/>
+      <c r="A43" s="137"/>
+      <c r="B43" s="126"/>
+      <c r="C43" s="129"/>
       <c r="D43" s="26">
         <v>0</v>
       </c>
@@ -4599,9 +4637,9 @@
       <c r="BE43" s="17"/>
     </row>
     <row r="44" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A44" s="93"/>
-      <c r="B44" s="120"/>
-      <c r="C44" s="105" t="s">
+      <c r="A44" s="137"/>
+      <c r="B44" s="126"/>
+      <c r="C44" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="25" t="s">
@@ -4618,48 +4656,48 @@
       <c r="V44" s="7"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="124"/>
-      <c r="Z44" s="124"/>
-      <c r="AA44" s="124"/>
-      <c r="AB44" s="124"/>
-      <c r="AC44" s="124"/>
+      <c r="Y44" s="92"/>
+      <c r="Z44" s="92"/>
+      <c r="AA44" s="92"/>
+      <c r="AB44" s="92"/>
+      <c r="AC44" s="92"/>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
-      <c r="AF44" s="124"/>
-      <c r="AG44" s="124"/>
-      <c r="AH44" s="124"/>
-      <c r="AI44" s="124"/>
-      <c r="AJ44" s="124"/>
+      <c r="AF44" s="92"/>
+      <c r="AG44" s="92"/>
+      <c r="AH44" s="92"/>
+      <c r="AI44" s="92"/>
+      <c r="AJ44" s="92"/>
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
-      <c r="AM44" s="124"/>
-      <c r="AN44" s="124"/>
-      <c r="AO44" s="129" t="s">
+      <c r="AM44" s="92"/>
+      <c r="AN44" s="92"/>
+      <c r="AO44" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="AP44" s="124" t="s">
+      <c r="AP44" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="AQ44" s="124"/>
+      <c r="AQ44" s="92"/>
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
-      <c r="AT44" s="124"/>
-      <c r="AU44" s="124"/>
-      <c r="AV44" s="124"/>
-      <c r="AW44" s="124"/>
-      <c r="AX44" s="124"/>
+      <c r="AT44" s="92"/>
+      <c r="AU44" s="92"/>
+      <c r="AV44" s="92"/>
+      <c r="AW44" s="92"/>
+      <c r="AX44" s="92"/>
       <c r="AY44" s="3"/>
       <c r="AZ44" s="3"/>
       <c r="BA44" s="7"/>
-      <c r="BB44" s="124"/>
-      <c r="BC44" s="124"/>
-      <c r="BD44" s="124"/>
+      <c r="BB44" s="92"/>
+      <c r="BC44" s="92"/>
+      <c r="BD44" s="92"/>
       <c r="BE44" s="8"/>
     </row>
     <row r="45" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A45" s="93"/>
-      <c r="B45" s="120"/>
-      <c r="C45" s="105"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="129"/>
       <c r="D45" s="26">
         <v>0</v>
       </c>
@@ -4720,9 +4758,9 @@
       <c r="BE45" s="17"/>
     </row>
     <row r="46" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A46" s="93"/>
-      <c r="B46" s="106"/>
-      <c r="C46" s="107"/>
+      <c r="A46" s="137"/>
+      <c r="B46" s="124"/>
+      <c r="C46" s="125"/>
       <c r="D46" s="79"/>
       <c r="E46" s="59"/>
       <c r="F46" s="28"/>
@@ -4779,8 +4817,8 @@
       <c r="BE46" s="30"/>
     </row>
     <row r="47" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A47" s="93"/>
-      <c r="B47" s="103" t="s">
+      <c r="A47" s="137"/>
+      <c r="B47" s="153" t="s">
         <v>43</v>
       </c>
       <c r="C47" s="48"/>
@@ -4821,7 +4859,7 @@
       <c r="AL47" s="32"/>
       <c r="AM47" s="32"/>
       <c r="AN47" s="32"/>
-      <c r="AO47" s="135"/>
+      <c r="AO47" s="102"/>
       <c r="AP47" s="32"/>
       <c r="AQ47" s="32"/>
       <c r="AR47" s="32"/>
@@ -4837,12 +4875,12 @@
       <c r="BB47" s="32"/>
       <c r="BC47" s="32"/>
       <c r="BD47" s="32"/>
-      <c r="BE47" s="142"/>
+      <c r="BE47" s="106"/>
     </row>
     <row r="48" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A48" s="93"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="105" t="s">
+      <c r="A48" s="137"/>
+      <c r="B48" s="153"/>
+      <c r="C48" s="129" t="s">
         <v>43</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -4859,52 +4897,52 @@
       <c r="Q48" s="3"/>
       <c r="S48" s="33"/>
       <c r="T48" s="33"/>
-      <c r="U48" s="126"/>
+      <c r="U48" s="94"/>
       <c r="V48" s="7"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="124"/>
-      <c r="Z48" s="124"/>
-      <c r="AA48" s="124"/>
-      <c r="AB48" s="124"/>
-      <c r="AC48" s="124"/>
+      <c r="Y48" s="92"/>
+      <c r="Z48" s="92"/>
+      <c r="AA48" s="92"/>
+      <c r="AB48" s="92"/>
+      <c r="AC48" s="92"/>
       <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
-      <c r="AF48" s="124"/>
-      <c r="AG48" s="124"/>
-      <c r="AH48" s="124"/>
-      <c r="AI48" s="124"/>
-      <c r="AJ48" s="124"/>
+      <c r="AF48" s="92"/>
+      <c r="AG48" s="92"/>
+      <c r="AH48" s="92"/>
+      <c r="AI48" s="92"/>
+      <c r="AJ48" s="92"/>
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
-      <c r="AM48" s="124"/>
-      <c r="AN48" s="124"/>
-      <c r="AO48" s="129"/>
-      <c r="AP48" s="125" t="s">
+      <c r="AM48" s="92"/>
+      <c r="AN48" s="92"/>
+      <c r="AO48" s="96"/>
+      <c r="AP48" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="AQ48" s="125" t="s">
+      <c r="AQ48" s="93" t="s">
         <v>44</v>
       </c>
       <c r="AR48" s="3"/>
       <c r="AS48" s="3"/>
-      <c r="AT48" s="124"/>
-      <c r="AU48" s="124"/>
-      <c r="AV48" s="124"/>
-      <c r="AW48" s="124"/>
-      <c r="AX48" s="124"/>
+      <c r="AT48" s="92"/>
+      <c r="AU48" s="92"/>
+      <c r="AV48" s="92"/>
+      <c r="AW48" s="92"/>
+      <c r="AX48" s="92"/>
       <c r="AY48" s="3"/>
       <c r="AZ48" s="3"/>
       <c r="BA48" s="7"/>
-      <c r="BB48" s="124"/>
-      <c r="BC48" s="124"/>
-      <c r="BD48" s="124"/>
+      <c r="BB48" s="92"/>
+      <c r="BC48" s="92"/>
+      <c r="BD48" s="92"/>
       <c r="BE48" s="8"/>
     </row>
     <row r="49" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="A49" s="93"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="105"/>
+      <c r="A49" s="137"/>
+      <c r="B49" s="153"/>
+      <c r="C49" s="129"/>
       <c r="D49" s="26">
         <v>0</v>
       </c>
@@ -4969,9 +5007,9 @@
       <c r="BE49" s="17"/>
     </row>
     <row r="50" spans="1:57" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="93"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="105" t="s">
+      <c r="A50" s="137"/>
+      <c r="B50" s="153"/>
+      <c r="C50" s="129" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="25" t="s">
@@ -4988,58 +5026,58 @@
       <c r="Q50" s="3"/>
       <c r="S50" s="33"/>
       <c r="T50" s="33"/>
-      <c r="U50" s="126"/>
+      <c r="U50" s="94"/>
       <c r="V50" s="7"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="124"/>
-      <c r="Z50" s="124"/>
-      <c r="AA50" s="124"/>
-      <c r="AB50" s="124"/>
-      <c r="AC50" s="124"/>
+      <c r="Y50" s="92"/>
+      <c r="Z50" s="92"/>
+      <c r="AA50" s="92"/>
+      <c r="AB50" s="92"/>
+      <c r="AC50" s="92"/>
       <c r="AD50" s="3"/>
       <c r="AE50" s="3"/>
-      <c r="AF50" s="124"/>
-      <c r="AG50" s="124"/>
-      <c r="AH50" s="124"/>
-      <c r="AI50" s="124"/>
-      <c r="AJ50" s="124"/>
+      <c r="AF50" s="92"/>
+      <c r="AG50" s="92"/>
+      <c r="AH50" s="92"/>
+      <c r="AI50" s="92"/>
+      <c r="AJ50" s="92"/>
       <c r="AK50" s="3"/>
       <c r="AL50" s="3"/>
-      <c r="AM50" s="124"/>
-      <c r="AN50" s="124"/>
-      <c r="AO50" s="129"/>
-      <c r="AP50" s="124"/>
-      <c r="AQ50" s="124"/>
+      <c r="AM50" s="92"/>
+      <c r="AN50" s="92"/>
+      <c r="AO50" s="96"/>
+      <c r="AP50" s="92"/>
+      <c r="AQ50" s="92"/>
       <c r="AR50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AS50" s="3"/>
-      <c r="AT50" s="125" t="s">
+      <c r="AT50" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="AU50" s="125"/>
-      <c r="AV50" s="125" t="s">
+      <c r="AU50" s="93"/>
+      <c r="AV50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="AW50" s="125" t="s">
+      <c r="AW50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="AX50" s="125" t="s">
+      <c r="AX50" s="93" t="s">
         <v>45</v>
       </c>
       <c r="AY50" s="3"/>
       <c r="AZ50" s="3"/>
-      <c r="BA50" s="132" t="s">
+      <c r="BA50" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="BB50" s="125" t="s">
+      <c r="BB50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="BC50" s="125" t="s">
+      <c r="BC50" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="BD50" s="125" t="s">
+      <c r="BD50" s="93" t="s">
         <v>45</v>
       </c>
       <c r="BE50" s="81" t="s">
@@ -5047,9 +5085,9 @@
       </c>
     </row>
     <row r="51" spans="1:57" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="93"/>
-      <c r="B51" s="103"/>
-      <c r="C51" s="105"/>
+      <c r="A51" s="137"/>
+      <c r="B51" s="153"/>
+      <c r="C51" s="129"/>
       <c r="D51" s="26">
         <v>0</v>
       </c>
@@ -5096,24 +5134,24 @@
       <c r="AQ51" s="2"/>
       <c r="AR51" s="2"/>
       <c r="AS51" s="2"/>
-      <c r="AT51" s="134"/>
-      <c r="AU51" s="134"/>
-      <c r="AV51" s="134"/>
-      <c r="AW51" s="134"/>
-      <c r="AX51" s="134"/>
+      <c r="AT51" s="101"/>
+      <c r="AU51" s="101"/>
+      <c r="AV51" s="101"/>
+      <c r="AW51" s="101"/>
+      <c r="AX51" s="101"/>
       <c r="AY51" s="3"/>
       <c r="AZ51" s="3"/>
-      <c r="BA51" s="143"/>
-      <c r="BB51" s="134"/>
-      <c r="BC51" s="134"/>
-      <c r="BD51" s="134"/>
+      <c r="BA51" s="107"/>
+      <c r="BB51" s="101"/>
+      <c r="BC51" s="101"/>
+      <c r="BD51" s="101"/>
       <c r="BE51" s="86">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="94"/>
-      <c r="B52" s="104"/>
+      <c r="A52" s="138"/>
+      <c r="B52" s="154"/>
       <c r="C52" s="68"/>
       <c r="D52" s="55"/>
       <c r="E52" s="69"/>
@@ -5164,103 +5202,103 @@
       <c r="AX52" s="71"/>
       <c r="AY52" s="71"/>
       <c r="AZ52" s="71"/>
-      <c r="BA52" s="144"/>
-      <c r="BB52" s="140"/>
-      <c r="BC52" s="140"/>
-      <c r="BD52" s="140"/>
-      <c r="BE52" s="141"/>
+      <c r="BA52" s="108"/>
+      <c r="BB52" s="104"/>
+      <c r="BC52" s="104"/>
+      <c r="BD52" s="104"/>
+      <c r="BE52" s="105"/>
     </row>
     <row r="53" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT53" s="152" t="s">
+      <c r="AT53" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="AU53" s="151"/>
-      <c r="AV53" s="151"/>
-      <c r="AW53" s="151"/>
-      <c r="AX53" s="151"/>
-      <c r="AY53" s="151"/>
-      <c r="AZ53" s="151"/>
-      <c r="BA53" s="151"/>
-      <c r="BB53" s="151"/>
-      <c r="BC53" s="151"/>
-      <c r="BD53" s="151"/>
-      <c r="BE53" s="109"/>
+      <c r="AU53" s="114"/>
+      <c r="AV53" s="114"/>
+      <c r="AW53" s="114"/>
+      <c r="AX53" s="114"/>
+      <c r="AY53" s="114"/>
+      <c r="AZ53" s="114"/>
+      <c r="BA53" s="114"/>
+      <c r="BB53" s="114"/>
+      <c r="BC53" s="114"/>
+      <c r="BD53" s="114"/>
+      <c r="BE53" s="115"/>
     </row>
     <row r="54" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q54" s="84"/>
       <c r="R54" s="84"/>
       <c r="S54" s="84"/>
-      <c r="AT54" s="110"/>
-      <c r="AU54" s="153"/>
-      <c r="AV54" s="153"/>
-      <c r="AW54" s="153"/>
-      <c r="AX54" s="153"/>
-      <c r="AY54" s="153"/>
-      <c r="AZ54" s="153"/>
-      <c r="BA54" s="153"/>
-      <c r="BB54" s="153"/>
-      <c r="BC54" s="153"/>
-      <c r="BD54" s="153"/>
-      <c r="BE54" s="111"/>
+      <c r="AT54" s="116"/>
+      <c r="AU54" s="117"/>
+      <c r="AV54" s="117"/>
+      <c r="AW54" s="117"/>
+      <c r="AX54" s="117"/>
+      <c r="AY54" s="117"/>
+      <c r="AZ54" s="117"/>
+      <c r="BA54" s="117"/>
+      <c r="BB54" s="117"/>
+      <c r="BC54" s="117"/>
+      <c r="BD54" s="117"/>
+      <c r="BE54" s="118"/>
     </row>
     <row r="55" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q55" s="84"/>
       <c r="R55" s="84"/>
       <c r="S55" s="84"/>
-      <c r="AT55" s="110"/>
-      <c r="AU55" s="153"/>
-      <c r="AV55" s="153"/>
-      <c r="AW55" s="153"/>
-      <c r="AX55" s="153"/>
-      <c r="AY55" s="153"/>
-      <c r="AZ55" s="153"/>
-      <c r="BA55" s="153"/>
-      <c r="BB55" s="153"/>
-      <c r="BC55" s="153"/>
-      <c r="BD55" s="153"/>
-      <c r="BE55" s="111"/>
+      <c r="AT55" s="116"/>
+      <c r="AU55" s="117"/>
+      <c r="AV55" s="117"/>
+      <c r="AW55" s="117"/>
+      <c r="AX55" s="117"/>
+      <c r="AY55" s="117"/>
+      <c r="AZ55" s="117"/>
+      <c r="BA55" s="117"/>
+      <c r="BB55" s="117"/>
+      <c r="BC55" s="117"/>
+      <c r="BD55" s="117"/>
+      <c r="BE55" s="118"/>
     </row>
     <row r="56" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT56" s="110"/>
-      <c r="AU56" s="153"/>
-      <c r="AV56" s="153"/>
-      <c r="AW56" s="153"/>
-      <c r="AX56" s="153"/>
-      <c r="AY56" s="153"/>
-      <c r="AZ56" s="153"/>
-      <c r="BA56" s="153"/>
-      <c r="BB56" s="153"/>
-      <c r="BC56" s="153"/>
-      <c r="BD56" s="153"/>
-      <c r="BE56" s="111"/>
+      <c r="AT56" s="116"/>
+      <c r="AU56" s="117"/>
+      <c r="AV56" s="117"/>
+      <c r="AW56" s="117"/>
+      <c r="AX56" s="117"/>
+      <c r="AY56" s="117"/>
+      <c r="AZ56" s="117"/>
+      <c r="BA56" s="117"/>
+      <c r="BB56" s="117"/>
+      <c r="BC56" s="117"/>
+      <c r="BD56" s="117"/>
+      <c r="BE56" s="118"/>
     </row>
     <row r="57" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AT57" s="110"/>
-      <c r="AU57" s="153"/>
-      <c r="AV57" s="153"/>
-      <c r="AW57" s="153"/>
-      <c r="AX57" s="153"/>
-      <c r="AY57" s="153"/>
-      <c r="AZ57" s="153"/>
-      <c r="BA57" s="153"/>
-      <c r="BB57" s="153"/>
-      <c r="BC57" s="153"/>
-      <c r="BD57" s="153"/>
-      <c r="BE57" s="111"/>
+      <c r="AT57" s="116"/>
+      <c r="AU57" s="117"/>
+      <c r="AV57" s="117"/>
+      <c r="AW57" s="117"/>
+      <c r="AX57" s="117"/>
+      <c r="AY57" s="117"/>
+      <c r="AZ57" s="117"/>
+      <c r="BA57" s="117"/>
+      <c r="BB57" s="117"/>
+      <c r="BC57" s="117"/>
+      <c r="BD57" s="117"/>
+      <c r="BE57" s="118"/>
     </row>
     <row r="58" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AT58" s="110"/>
-      <c r="AU58" s="153"/>
-      <c r="AV58" s="153"/>
-      <c r="AW58" s="153"/>
-      <c r="AX58" s="153"/>
-      <c r="AY58" s="153"/>
-      <c r="AZ58" s="153"/>
-      <c r="BA58" s="153"/>
-      <c r="BB58" s="153"/>
-      <c r="BC58" s="153"/>
-      <c r="BD58" s="153"/>
-      <c r="BE58" s="111"/>
+      <c r="AT58" s="116"/>
+      <c r="AU58" s="117"/>
+      <c r="AV58" s="117"/>
+      <c r="AW58" s="117"/>
+      <c r="AX58" s="117"/>
+      <c r="AY58" s="117"/>
+      <c r="AZ58" s="117"/>
+      <c r="BA58" s="117"/>
+      <c r="BB58" s="117"/>
+      <c r="BC58" s="117"/>
+      <c r="BD58" s="117"/>
+      <c r="BE58" s="118"/>
     </row>
     <row r="59" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A59" s="40" t="s">
@@ -5273,18 +5311,25 @@
       <c r="D59" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AT59" s="110"/>
-      <c r="AU59" s="153"/>
-      <c r="AV59" s="153"/>
-      <c r="AW59" s="153"/>
-      <c r="AX59" s="153"/>
-      <c r="AY59" s="153"/>
-      <c r="AZ59" s="153"/>
-      <c r="BA59" s="153"/>
-      <c r="BB59" s="153"/>
-      <c r="BC59" s="153"/>
-      <c r="BD59" s="153"/>
-      <c r="BE59" s="111"/>
+      <c r="AO59" s="161" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP59" s="114"/>
+      <c r="AQ59" s="114"/>
+      <c r="AR59" s="114"/>
+      <c r="AS59" s="115"/>
+      <c r="AT59" s="116"/>
+      <c r="AU59" s="117"/>
+      <c r="AV59" s="117"/>
+      <c r="AW59" s="117"/>
+      <c r="AX59" s="117"/>
+      <c r="AY59" s="117"/>
+      <c r="AZ59" s="117"/>
+      <c r="BA59" s="117"/>
+      <c r="BB59" s="117"/>
+      <c r="BC59" s="117"/>
+      <c r="BD59" s="117"/>
+      <c r="BE59" s="118"/>
     </row>
     <row r="60" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A60" s="41"/>
@@ -5295,18 +5340,23 @@
       <c r="D60" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AT60" s="110"/>
-      <c r="AU60" s="153"/>
-      <c r="AV60" s="153"/>
-      <c r="AW60" s="153"/>
-      <c r="AX60" s="153"/>
-      <c r="AY60" s="153"/>
-      <c r="AZ60" s="153"/>
-      <c r="BA60" s="153"/>
-      <c r="BB60" s="153"/>
-      <c r="BC60" s="153"/>
-      <c r="BD60" s="153"/>
-      <c r="BE60" s="111"/>
+      <c r="AO60" s="116"/>
+      <c r="AP60" s="117"/>
+      <c r="AQ60" s="117"/>
+      <c r="AR60" s="117"/>
+      <c r="AS60" s="118"/>
+      <c r="AT60" s="116"/>
+      <c r="AU60" s="117"/>
+      <c r="AV60" s="117"/>
+      <c r="AW60" s="117"/>
+      <c r="AX60" s="117"/>
+      <c r="AY60" s="117"/>
+      <c r="AZ60" s="117"/>
+      <c r="BA60" s="117"/>
+      <c r="BB60" s="117"/>
+      <c r="BC60" s="117"/>
+      <c r="BD60" s="117"/>
+      <c r="BE60" s="118"/>
     </row>
     <row r="61" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A61" s="41" t="s">
@@ -5321,18 +5371,23 @@
       <c r="D61" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AT61" s="110"/>
-      <c r="AU61" s="153"/>
-      <c r="AV61" s="153"/>
-      <c r="AW61" s="153"/>
-      <c r="AX61" s="153"/>
-      <c r="AY61" s="153"/>
-      <c r="AZ61" s="153"/>
-      <c r="BA61" s="153"/>
-      <c r="BB61" s="153"/>
-      <c r="BC61" s="153"/>
-      <c r="BD61" s="153"/>
-      <c r="BE61" s="111"/>
+      <c r="AO61" s="116"/>
+      <c r="AP61" s="117"/>
+      <c r="AQ61" s="117"/>
+      <c r="AR61" s="117"/>
+      <c r="AS61" s="118"/>
+      <c r="AT61" s="116"/>
+      <c r="AU61" s="117"/>
+      <c r="AV61" s="117"/>
+      <c r="AW61" s="117"/>
+      <c r="AX61" s="117"/>
+      <c r="AY61" s="117"/>
+      <c r="AZ61" s="117"/>
+      <c r="BA61" s="117"/>
+      <c r="BB61" s="117"/>
+      <c r="BC61" s="117"/>
+      <c r="BD61" s="117"/>
+      <c r="BE61" s="118"/>
     </row>
     <row r="62" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A62" s="41"/>
@@ -5345,18 +5400,23 @@
       <c r="D62" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AT62" s="110"/>
-      <c r="AU62" s="153"/>
-      <c r="AV62" s="153"/>
-      <c r="AW62" s="153"/>
-      <c r="AX62" s="153"/>
-      <c r="AY62" s="153"/>
-      <c r="AZ62" s="153"/>
-      <c r="BA62" s="153"/>
-      <c r="BB62" s="153"/>
-      <c r="BC62" s="153"/>
-      <c r="BD62" s="153"/>
-      <c r="BE62" s="111"/>
+      <c r="AO62" s="116"/>
+      <c r="AP62" s="117"/>
+      <c r="AQ62" s="117"/>
+      <c r="AR62" s="117"/>
+      <c r="AS62" s="118"/>
+      <c r="AT62" s="116"/>
+      <c r="AU62" s="117"/>
+      <c r="AV62" s="117"/>
+      <c r="AW62" s="117"/>
+      <c r="AX62" s="117"/>
+      <c r="AY62" s="117"/>
+      <c r="AZ62" s="117"/>
+      <c r="BA62" s="117"/>
+      <c r="BB62" s="117"/>
+      <c r="BC62" s="117"/>
+      <c r="BD62" s="117"/>
+      <c r="BE62" s="118"/>
     </row>
     <row r="63" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A63" s="41"/>
@@ -5369,20 +5429,25 @@
       <c r="D63" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AT63" s="110"/>
-      <c r="AU63" s="153"/>
-      <c r="AV63" s="153"/>
-      <c r="AW63" s="153"/>
-      <c r="AX63" s="153"/>
-      <c r="AY63" s="153"/>
-      <c r="AZ63" s="153"/>
-      <c r="BA63" s="153"/>
-      <c r="BB63" s="153"/>
-      <c r="BC63" s="153"/>
-      <c r="BD63" s="153"/>
-      <c r="BE63" s="111"/>
-    </row>
-    <row r="64" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="AO63" s="116"/>
+      <c r="AP63" s="117"/>
+      <c r="AQ63" s="117"/>
+      <c r="AR63" s="117"/>
+      <c r="AS63" s="118"/>
+      <c r="AT63" s="116"/>
+      <c r="AU63" s="117"/>
+      <c r="AV63" s="117"/>
+      <c r="AW63" s="117"/>
+      <c r="AX63" s="117"/>
+      <c r="AY63" s="117"/>
+      <c r="AZ63" s="117"/>
+      <c r="BA63" s="117"/>
+      <c r="BB63" s="117"/>
+      <c r="BC63" s="117"/>
+      <c r="BD63" s="117"/>
+      <c r="BE63" s="118"/>
+    </row>
+    <row r="64" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
       <c r="B64" s="23" t="s">
         <v>47</v>
@@ -5393,18 +5458,23 @@
       <c r="D64" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AT64" s="110"/>
-      <c r="AU64" s="153"/>
-      <c r="AV64" s="153"/>
-      <c r="AW64" s="153"/>
-      <c r="AX64" s="153"/>
-      <c r="AY64" s="153"/>
-      <c r="AZ64" s="153"/>
-      <c r="BA64" s="153"/>
-      <c r="BB64" s="153"/>
-      <c r="BC64" s="153"/>
-      <c r="BD64" s="153"/>
-      <c r="BE64" s="111"/>
+      <c r="AO64" s="119"/>
+      <c r="AP64" s="120"/>
+      <c r="AQ64" s="120"/>
+      <c r="AR64" s="120"/>
+      <c r="AS64" s="121"/>
+      <c r="AT64" s="116"/>
+      <c r="AU64" s="117"/>
+      <c r="AV64" s="117"/>
+      <c r="AW64" s="117"/>
+      <c r="AX64" s="117"/>
+      <c r="AY64" s="117"/>
+      <c r="AZ64" s="117"/>
+      <c r="BA64" s="117"/>
+      <c r="BB64" s="117"/>
+      <c r="BC64" s="117"/>
+      <c r="BD64" s="117"/>
+      <c r="BE64" s="118"/>
     </row>
     <row r="65" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A65" s="41"/>
@@ -5417,18 +5487,18 @@
       <c r="D65" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AT65" s="110"/>
-      <c r="AU65" s="153"/>
-      <c r="AV65" s="153"/>
-      <c r="AW65" s="153"/>
-      <c r="AX65" s="153"/>
-      <c r="AY65" s="153"/>
-      <c r="AZ65" s="153"/>
-      <c r="BA65" s="153"/>
-      <c r="BB65" s="153"/>
-      <c r="BC65" s="153"/>
-      <c r="BD65" s="153"/>
-      <c r="BE65" s="111"/>
+      <c r="AT65" s="116"/>
+      <c r="AU65" s="117"/>
+      <c r="AV65" s="117"/>
+      <c r="AW65" s="117"/>
+      <c r="AX65" s="117"/>
+      <c r="AY65" s="117"/>
+      <c r="AZ65" s="117"/>
+      <c r="BA65" s="117"/>
+      <c r="BB65" s="117"/>
+      <c r="BC65" s="117"/>
+      <c r="BD65" s="117"/>
+      <c r="BE65" s="118"/>
     </row>
     <row r="66" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A66" s="41"/>
@@ -5437,36 +5507,36 @@
       <c r="D66" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AT66" s="110"/>
-      <c r="AU66" s="153"/>
-      <c r="AV66" s="153"/>
-      <c r="AW66" s="153"/>
-      <c r="AX66" s="153"/>
-      <c r="AY66" s="153"/>
-      <c r="AZ66" s="153"/>
-      <c r="BA66" s="153"/>
-      <c r="BB66" s="153"/>
-      <c r="BC66" s="153"/>
-      <c r="BD66" s="153"/>
-      <c r="BE66" s="111"/>
+      <c r="AT66" s="116"/>
+      <c r="AU66" s="117"/>
+      <c r="AV66" s="117"/>
+      <c r="AW66" s="117"/>
+      <c r="AX66" s="117"/>
+      <c r="AY66" s="117"/>
+      <c r="AZ66" s="117"/>
+      <c r="BA66" s="117"/>
+      <c r="BB66" s="117"/>
+      <c r="BC66" s="117"/>
+      <c r="BD66" s="117"/>
+      <c r="BE66" s="118"/>
     </row>
     <row r="67" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A67" s="41"/>
       <c r="B67" s="23"/>
       <c r="C67" s="14"/>
       <c r="D67" s="9"/>
-      <c r="AT67" s="110"/>
-      <c r="AU67" s="153"/>
-      <c r="AV67" s="153"/>
-      <c r="AW67" s="153"/>
-      <c r="AX67" s="153"/>
-      <c r="AY67" s="153"/>
-      <c r="AZ67" s="153"/>
-      <c r="BA67" s="153"/>
-      <c r="BB67" s="153"/>
-      <c r="BC67" s="153"/>
-      <c r="BD67" s="153"/>
-      <c r="BE67" s="111"/>
+      <c r="AT67" s="116"/>
+      <c r="AU67" s="117"/>
+      <c r="AV67" s="117"/>
+      <c r="AW67" s="117"/>
+      <c r="AX67" s="117"/>
+      <c r="AY67" s="117"/>
+      <c r="AZ67" s="117"/>
+      <c r="BA67" s="117"/>
+      <c r="BB67" s="117"/>
+      <c r="BC67" s="117"/>
+      <c r="BD67" s="117"/>
+      <c r="BE67" s="118"/>
     </row>
     <row r="68" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A68" s="41" t="s">
@@ -5479,36 +5549,36 @@
       <c r="D68" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AT68" s="110"/>
-      <c r="AU68" s="153"/>
-      <c r="AV68" s="153"/>
-      <c r="AW68" s="153"/>
-      <c r="AX68" s="153"/>
-      <c r="AY68" s="153"/>
-      <c r="AZ68" s="153"/>
-      <c r="BA68" s="153"/>
-      <c r="BB68" s="153"/>
-      <c r="BC68" s="153"/>
-      <c r="BD68" s="153"/>
-      <c r="BE68" s="111"/>
+      <c r="AT68" s="116"/>
+      <c r="AU68" s="117"/>
+      <c r="AV68" s="117"/>
+      <c r="AW68" s="117"/>
+      <c r="AX68" s="117"/>
+      <c r="AY68" s="117"/>
+      <c r="AZ68" s="117"/>
+      <c r="BA68" s="117"/>
+      <c r="BB68" s="117"/>
+      <c r="BC68" s="117"/>
+      <c r="BD68" s="117"/>
+      <c r="BE68" s="118"/>
     </row>
     <row r="69" spans="1:57" ht="13.2" x14ac:dyDescent="0.2">
       <c r="A69" s="41"/>
       <c r="B69" s="23"/>
       <c r="C69" s="14"/>
       <c r="D69" s="9"/>
-      <c r="AT69" s="110"/>
-      <c r="AU69" s="153"/>
-      <c r="AV69" s="153"/>
-      <c r="AW69" s="153"/>
-      <c r="AX69" s="153"/>
-      <c r="AY69" s="153"/>
-      <c r="AZ69" s="153"/>
-      <c r="BA69" s="153"/>
-      <c r="BB69" s="153"/>
-      <c r="BC69" s="153"/>
-      <c r="BD69" s="153"/>
-      <c r="BE69" s="111"/>
+      <c r="AT69" s="116"/>
+      <c r="AU69" s="117"/>
+      <c r="AV69" s="117"/>
+      <c r="AW69" s="117"/>
+      <c r="AX69" s="117"/>
+      <c r="AY69" s="117"/>
+      <c r="AZ69" s="117"/>
+      <c r="BA69" s="117"/>
+      <c r="BB69" s="117"/>
+      <c r="BC69" s="117"/>
+      <c r="BD69" s="117"/>
+      <c r="BE69" s="118"/>
     </row>
     <row r="70" spans="1:57" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="42" t="s">
@@ -5521,58 +5591,264 @@
       <c r="D70" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="AT70" s="112"/>
-      <c r="AU70" s="154"/>
-      <c r="AV70" s="154"/>
-      <c r="AW70" s="154"/>
-      <c r="AX70" s="154"/>
-      <c r="AY70" s="154"/>
-      <c r="AZ70" s="154"/>
-      <c r="BA70" s="154"/>
-      <c r="BB70" s="154"/>
-      <c r="BC70" s="154"/>
-      <c r="BD70" s="154"/>
-      <c r="BE70" s="113"/>
-    </row>
-    <row r="75" spans="1:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+      <c r="AT70" s="119"/>
+      <c r="AU70" s="120"/>
+      <c r="AV70" s="120"/>
+      <c r="AW70" s="120"/>
+      <c r="AX70" s="120"/>
+      <c r="AY70" s="120"/>
+      <c r="AZ70" s="120"/>
+      <c r="BA70" s="120"/>
+      <c r="BB70" s="120"/>
+      <c r="BC70" s="120"/>
+      <c r="BD70" s="120"/>
+      <c r="BE70" s="121"/>
+    </row>
+    <row r="71" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT71" s="155"/>
+      <c r="AU71" s="156"/>
+      <c r="AV71" s="156"/>
+      <c r="AW71" s="156"/>
+      <c r="AX71" s="156"/>
+      <c r="AY71" s="156"/>
+      <c r="AZ71" s="156"/>
+      <c r="BA71" s="156"/>
+      <c r="BB71" s="156"/>
+      <c r="BC71" s="156"/>
+      <c r="BD71" s="156"/>
+      <c r="BE71" s="157"/>
+    </row>
+    <row r="72" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT72" s="7"/>
+      <c r="AU72" s="92"/>
+      <c r="AV72" s="92"/>
+      <c r="AW72" s="92"/>
+      <c r="AX72" s="92"/>
+      <c r="AY72" s="92"/>
+      <c r="AZ72" s="92"/>
+      <c r="BA72" s="92"/>
+      <c r="BB72" s="92"/>
+      <c r="BC72" s="92"/>
+      <c r="BD72" s="92"/>
+      <c r="BE72" s="8"/>
+    </row>
+    <row r="73" spans="1:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AT73" s="7"/>
+      <c r="AU73" s="92"/>
+      <c r="AV73" s="92"/>
+      <c r="AW73" s="92"/>
+      <c r="AX73" s="92"/>
+      <c r="AY73" s="92"/>
+      <c r="AZ73" s="92"/>
+      <c r="BA73" s="92"/>
+      <c r="BB73" s="92"/>
+      <c r="BC73" s="92"/>
+      <c r="BD73" s="92"/>
+      <c r="BE73" s="8"/>
+    </row>
+    <row r="74" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AO74" s="161" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP74" s="114"/>
+      <c r="AQ74" s="114"/>
+      <c r="AR74" s="114"/>
+      <c r="AS74" s="114"/>
+      <c r="AT74" s="7"/>
+      <c r="AU74" s="92"/>
+      <c r="AV74" s="92"/>
+      <c r="AW74" s="92"/>
+      <c r="AX74" s="92"/>
+      <c r="AY74" s="92"/>
+      <c r="AZ74" s="92"/>
+      <c r="BA74" s="92"/>
+      <c r="BB74" s="92"/>
+      <c r="BC74" s="92"/>
+      <c r="BD74" s="92"/>
+      <c r="BE74" s="8"/>
+    </row>
+    <row r="75" spans="1:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO75" s="116"/>
+      <c r="AP75" s="117"/>
+      <c r="AQ75" s="117"/>
+      <c r="AR75" s="117"/>
+      <c r="AS75" s="117"/>
+      <c r="AT75" s="7"/>
+      <c r="AU75" s="92"/>
+      <c r="AV75" s="92"/>
+      <c r="AW75" s="92"/>
+      <c r="AX75" s="92"/>
+      <c r="AY75" s="92"/>
+      <c r="AZ75" s="92"/>
+      <c r="BA75" s="92"/>
+      <c r="BB75" s="92"/>
+      <c r="BC75" s="92"/>
+      <c r="BD75" s="92"/>
+      <c r="BE75" s="8"/>
+    </row>
     <row r="76" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="34" t="s">
         <v>0</v>
       </c>
+      <c r="AO76" s="116"/>
+      <c r="AP76" s="117"/>
+      <c r="AQ76" s="117"/>
+      <c r="AR76" s="117"/>
+      <c r="AS76" s="117"/>
+      <c r="AT76" s="7"/>
+      <c r="AU76" s="92"/>
+      <c r="AV76" s="92"/>
+      <c r="AW76" s="92"/>
+      <c r="AX76" s="92"/>
+      <c r="AY76" s="92"/>
+      <c r="AZ76" s="92"/>
+      <c r="BA76" s="92"/>
+      <c r="BB76" s="92"/>
+      <c r="BC76" s="92"/>
+      <c r="BD76" s="92"/>
+      <c r="BE76" s="8"/>
     </row>
     <row r="77" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="35" t="s">
         <v>2</v>
       </c>
+      <c r="AO77" s="116"/>
+      <c r="AP77" s="117"/>
+      <c r="AQ77" s="117"/>
+      <c r="AR77" s="117"/>
+      <c r="AS77" s="117"/>
+      <c r="AT77" s="7"/>
+      <c r="AU77" s="92"/>
+      <c r="AV77" s="92"/>
+      <c r="AW77" s="92"/>
+      <c r="AX77" s="92"/>
+      <c r="AY77" s="92"/>
+      <c r="AZ77" s="92"/>
+      <c r="BA77" s="92"/>
+      <c r="BB77" s="92"/>
+      <c r="BC77" s="92"/>
+      <c r="BD77" s="92"/>
+      <c r="BE77" s="8"/>
     </row>
     <row r="78" spans="1:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="72" t="s">
         <v>3</v>
       </c>
+      <c r="AO78" s="116"/>
+      <c r="AP78" s="117"/>
+      <c r="AQ78" s="117"/>
+      <c r="AR78" s="117"/>
+      <c r="AS78" s="117"/>
+      <c r="AT78" s="7"/>
+      <c r="AU78" s="92"/>
+      <c r="AV78" s="92"/>
+      <c r="AW78" s="92"/>
+      <c r="AX78" s="92"/>
+      <c r="AY78" s="92"/>
+      <c r="AZ78" s="92"/>
+      <c r="BA78" s="92"/>
+      <c r="BB78" s="92"/>
+      <c r="BC78" s="92"/>
+      <c r="BD78" s="92"/>
+      <c r="BE78" s="8"/>
+    </row>
+    <row r="79" spans="1:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AO79" s="116"/>
+      <c r="AP79" s="117"/>
+      <c r="AQ79" s="117"/>
+      <c r="AR79" s="117"/>
+      <c r="AS79" s="117"/>
+      <c r="AT79" s="7"/>
+      <c r="AU79" s="92"/>
+      <c r="AV79" s="92"/>
+      <c r="AW79" s="92"/>
+      <c r="AX79" s="92"/>
+      <c r="AY79" s="92"/>
+      <c r="AZ79" s="92"/>
+      <c r="BA79" s="92"/>
+      <c r="BB79" s="92"/>
+      <c r="BC79" s="92"/>
+      <c r="BD79" s="92"/>
+      <c r="BE79" s="8"/>
+    </row>
+    <row r="80" spans="1:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO80" s="119"/>
+      <c r="AP80" s="120"/>
+      <c r="AQ80" s="120"/>
+      <c r="AR80" s="120"/>
+      <c r="AS80" s="120"/>
+      <c r="AT80" s="7"/>
+      <c r="AU80" s="92"/>
+      <c r="AV80" s="92"/>
+      <c r="AW80" s="92"/>
+      <c r="AX80" s="92"/>
+      <c r="AY80" s="92"/>
+      <c r="AZ80" s="92"/>
+      <c r="BA80" s="92"/>
+      <c r="BB80" s="92"/>
+      <c r="BC80" s="92"/>
+      <c r="BD80" s="92"/>
+      <c r="BE80" s="8"/>
+    </row>
+    <row r="81" spans="46:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT81" s="7"/>
+      <c r="AU81" s="92"/>
+      <c r="AV81" s="92"/>
+      <c r="AW81" s="92"/>
+      <c r="AX81" s="92"/>
+      <c r="AY81" s="92"/>
+      <c r="AZ81" s="92"/>
+      <c r="BA81" s="92"/>
+      <c r="BB81" s="92"/>
+      <c r="BC81" s="92"/>
+      <c r="BD81" s="92"/>
+      <c r="BE81" s="8"/>
+    </row>
+    <row r="82" spans="46:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT82" s="7"/>
+      <c r="AU82" s="92"/>
+      <c r="AV82" s="92"/>
+      <c r="AW82" s="92"/>
+      <c r="AX82" s="92"/>
+      <c r="AY82" s="92"/>
+      <c r="AZ82" s="92"/>
+      <c r="BA82" s="92"/>
+      <c r="BB82" s="92"/>
+      <c r="BC82" s="92"/>
+      <c r="BD82" s="92"/>
+      <c r="BE82" s="8"/>
+    </row>
+    <row r="83" spans="46:57" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AT83" s="7"/>
+      <c r="AU83" s="92"/>
+      <c r="AV83" s="92"/>
+      <c r="AW83" s="92"/>
+      <c r="AX83" s="92"/>
+      <c r="AY83" s="92"/>
+      <c r="AZ83" s="92"/>
+      <c r="BA83" s="92"/>
+      <c r="BB83" s="92"/>
+      <c r="BC83" s="92"/>
+      <c r="BD83" s="92"/>
+      <c r="BE83" s="8"/>
+    </row>
+    <row r="84" spans="46:57" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AT84" s="158"/>
+      <c r="AU84" s="159"/>
+      <c r="AV84" s="159"/>
+      <c r="AW84" s="159"/>
+      <c r="AX84" s="159"/>
+      <c r="AY84" s="159"/>
+      <c r="AZ84" s="159"/>
+      <c r="BA84" s="159"/>
+      <c r="BB84" s="159"/>
+      <c r="BC84" s="159"/>
+      <c r="BD84" s="159"/>
+      <c r="BE84" s="160"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="BA5:BE5"/>
-    <mergeCell ref="AT53:BE70"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B20:B39"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B1:C4"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B12:C12"/>
+  <mergeCells count="39">
+    <mergeCell ref="AO74:AS80"/>
     <mergeCell ref="A7:A52"/>
     <mergeCell ref="V5:AZ5"/>
     <mergeCell ref="A5:A6"/>
@@ -5589,6 +5865,28 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B1:C4"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="BA5:BE5"/>
+    <mergeCell ref="AT53:BE70"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B20:B39"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="AO59:AS64"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5597,15 +5895,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a281c49-7b6d-4f8c-afe3-9ff903bcd5b8">
@@ -5614,6 +5903,15 @@
     <TaxCatchAll xmlns="266e6b36-48df-40d6-b278-0c40cd134fd3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5852,14 +6150,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B2104E-3D92-4822-8BD9-D0FE6E4D87FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{352C3874-9B90-4780-AB48-A7AFE198EA9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -5872,6 +6162,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B2104E-3D92-4822-8BD9-D0FE6E4D87FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>